<commit_message>
membership details,set screenshot directory path,cross browser
</commit_message>
<xml_diff>
--- a/test_data/data.xlsx
+++ b/test_data/data.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddEmergencyContact" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="AddMemberships" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>${username}</t>
   </si>
@@ -47,13 +49,34 @@
   </si>
   <si>
     <t>Sister</t>
+  </si>
+  <si>
+    <t>${membership}</t>
+  </si>
+  <si>
+    <t>${coin}</t>
+  </si>
+  <si>
+    <t>ACCA</t>
+  </si>
+  <si>
+    <t>Indian Rupee</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>${amount}</t>
+  </si>
+  <si>
+    <t>${paid_by}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -64,6 +87,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -87,11 +117,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -304,7 +336,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -368,4 +400,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="6" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3">
+        <v>500</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>